<commit_message>
carga desde xlsx de profesores en bbdd
</commit_message>
<xml_diff>
--- a/web_app/public/plantillas/profesoresPlantilla.xlsx
+++ b/web_app/public/plantillas/profesoresPlantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TFG\TFG-PAP\web_app\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7309FD9A-322E-497D-A29D-A9298ABB8766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92778A5B-3FAD-4AB6-ACB0-230855053561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,13 @@
     <t>UVUS</t>
   </si>
   <si>
-    <t>Capacidad efectiva</t>
+    <t>Nombre</t>
   </si>
   <si>
-    <t>Apellidos, Nombre</t>
+    <t>Apellidos</t>
   </si>
   <si>
-    <t>PROFESORES</t>
+    <t>Capacidad</t>
   </si>
 </sst>
 </file>
@@ -89,11 +89,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -376,46 +373,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="20.77734375" customWidth="1"/>
+    <col min="1" max="5" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D11" s="3"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>